<commit_message>
Start Notebook for everyone's exploration
</commit_message>
<xml_diff>
--- a/Time_Tracking.xlsx
+++ b/Time_Tracking.xlsx
@@ -106,7 +106,7 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" mc:Ignorable="x14ac">
   <numFmts count="0"/>
-  <fonts count="7" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -145,12 +145,6 @@
       <b/>
       <sz val="12"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
     </font>
@@ -702,7 +696,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="58">
+  <cellXfs count="56">
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0"/>
     <xf xfId="0" numFmtId="0" borderId="0" fontId="0" fillId="0" applyAlignment="1">
       <alignment horizontal="general"/>
@@ -863,17 +857,11 @@
     <xf xfId="0" numFmtId="0" borderId="36" applyBorder="1" fontId="1" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="1" applyBorder="1" fontId="6" applyFont="1" fillId="0" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="17" applyBorder="1" fontId="3" applyFont="1" fillId="3" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="22" applyBorder="1" fontId="5" applyFont="1" fillId="4" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
-    </xf>
-    <xf xfId="0" numFmtId="4" applyNumberFormat="1" borderId="0" fontId="0" fillId="0" applyAlignment="1">
-      <alignment horizontal="general"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1245,7 +1233,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="54" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="28"/>
@@ -1275,7 +1263,7 @@
       <c r="C4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="55" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="35" t="s">
@@ -2859,7 +2847,7 @@
     <col min="1" max="1" style="20" width="13.576428571428572" customWidth="1" bestFit="1"/>
     <col min="2" max="2" style="51" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="3" max="3" style="52" width="13.576428571428572" customWidth="1" bestFit="1"/>
-    <col min="4" max="4" style="57" width="11.43357142857143" customWidth="1" bestFit="1"/>
+    <col min="4" max="4" style="22" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="5" max="5" style="20" width="22.862142857142857" customWidth="1" bestFit="1"/>
     <col min="6" max="6" style="20" width="11.43357142857143" customWidth="1" bestFit="1"/>
     <col min="7" max="7" style="20" width="22.862142857142857" customWidth="1" bestFit="1"/>
@@ -2874,11 +2862,11 @@
     <col min="16" max="16" style="22" width="13.576428571428572" customWidth="1" bestFit="1"/>
   </cols>
   <sheetData>
-    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="1" customHeight="1" ht="19.5">
       <c r="A1" s="1"/>
       <c r="B1" s="19"/>
       <c r="C1" s="23"/>
-      <c r="D1" s="54"/>
+      <c r="D1" s="3"/>
       <c r="E1" s="1"/>
       <c r="F1" s="1"/>
       <c r="G1" s="1"/>
@@ -2918,7 +2906,7 @@
         <v>14</v>
       </c>
       <c r="C3" s="28"/>
-      <c r="D3" s="55" t="s">
+      <c r="D3" s="54" t="s">
         <v>2</v>
       </c>
       <c r="E3" s="28"/>
@@ -2948,7 +2936,7 @@
       <c r="C4" s="33" t="s">
         <v>15</v>
       </c>
-      <c r="D4" s="56" t="s">
+      <c r="D4" s="55" t="s">
         <v>16</v>
       </c>
       <c r="E4" s="35" t="s">
@@ -3116,7 +3104,9 @@
       <c r="C10" s="42" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="11"/>
+      <c r="D10" s="11">
+        <v>3.5</v>
+      </c>
       <c r="E10" s="39"/>
       <c r="F10" s="11"/>
       <c r="G10" s="39"/>
@@ -3690,7 +3680,7 @@
       <c r="A36" s="1"/>
       <c r="B36" s="19"/>
       <c r="C36" s="23"/>
-      <c r="D36" s="54"/>
+      <c r="D36" s="3"/>
       <c r="E36" s="1"/>
       <c r="F36" s="1"/>
       <c r="G36" s="1"/>
@@ -3708,7 +3698,7 @@
       <c r="A37" s="1"/>
       <c r="B37" s="19"/>
       <c r="C37" s="23"/>
-      <c r="D37" s="54"/>
+      <c r="D37" s="3"/>
       <c r="E37" s="1"/>
       <c r="F37" s="1"/>
       <c r="G37" s="1"/>
@@ -3726,7 +3716,7 @@
       <c r="A38" s="1"/>
       <c r="B38" s="19"/>
       <c r="C38" s="23"/>
-      <c r="D38" s="54"/>
+      <c r="D38" s="3"/>
       <c r="E38" s="1"/>
       <c r="F38" s="1"/>
       <c r="G38" s="1"/>
@@ -3744,7 +3734,7 @@
       <c r="A39" s="1"/>
       <c r="B39" s="19"/>
       <c r="C39" s="23"/>
-      <c r="D39" s="54"/>
+      <c r="D39" s="3"/>
       <c r="E39" s="1"/>
       <c r="F39" s="1"/>
       <c r="G39" s="1"/>
@@ -3762,7 +3752,7 @@
       <c r="A40" s="1"/>
       <c r="B40" s="19"/>
       <c r="C40" s="23"/>
-      <c r="D40" s="54"/>
+      <c r="D40" s="3"/>
       <c r="E40" s="1"/>
       <c r="F40" s="1"/>
       <c r="G40" s="1"/>
@@ -3780,7 +3770,7 @@
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="23"/>
-      <c r="D41" s="54"/>
+      <c r="D41" s="3"/>
       <c r="E41" s="1"/>
       <c r="F41" s="1"/>
       <c r="G41" s="1"/>
@@ -3798,7 +3788,7 @@
       <c r="A42" s="1"/>
       <c r="B42" s="19"/>
       <c r="C42" s="23"/>
-      <c r="D42" s="54"/>
+      <c r="D42" s="3"/>
       <c r="E42" s="1"/>
       <c r="F42" s="1"/>
       <c r="G42" s="1"/>
@@ -3816,7 +3806,7 @@
       <c r="A43" s="1"/>
       <c r="B43" s="19"/>
       <c r="C43" s="23"/>
-      <c r="D43" s="54"/>
+      <c r="D43" s="3"/>
       <c r="E43" s="1"/>
       <c r="F43" s="1"/>
       <c r="G43" s="1"/>
@@ -3834,7 +3824,7 @@
       <c r="A44" s="1"/>
       <c r="B44" s="19"/>
       <c r="C44" s="23"/>
-      <c r="D44" s="54"/>
+      <c r="D44" s="3"/>
       <c r="E44" s="1"/>
       <c r="F44" s="1"/>
       <c r="G44" s="1"/>
@@ -3852,7 +3842,7 @@
       <c r="A45" s="1"/>
       <c r="B45" s="19"/>
       <c r="C45" s="23"/>
-      <c r="D45" s="54"/>
+      <c r="D45" s="3"/>
       <c r="E45" s="1"/>
       <c r="F45" s="1"/>
       <c r="G45" s="1"/>
@@ -3870,7 +3860,7 @@
       <c r="A46" s="1"/>
       <c r="B46" s="19"/>
       <c r="C46" s="23"/>
-      <c r="D46" s="54"/>
+      <c r="D46" s="3"/>
       <c r="E46" s="1"/>
       <c r="F46" s="1"/>
       <c r="G46" s="1"/>
@@ -3888,7 +3878,7 @@
       <c r="A47" s="1"/>
       <c r="B47" s="19"/>
       <c r="C47" s="23"/>
-      <c r="D47" s="54"/>
+      <c r="D47" s="3"/>
       <c r="E47" s="1"/>
       <c r="F47" s="1"/>
       <c r="G47" s="1"/>
@@ -3906,7 +3896,7 @@
       <c r="A48" s="1"/>
       <c r="B48" s="19"/>
       <c r="C48" s="23"/>
-      <c r="D48" s="54"/>
+      <c r="D48" s="3"/>
       <c r="E48" s="1"/>
       <c r="F48" s="1"/>
       <c r="G48" s="1"/>
@@ -3924,7 +3914,7 @@
       <c r="A49" s="1"/>
       <c r="B49" s="19"/>
       <c r="C49" s="23"/>
-      <c r="D49" s="54"/>
+      <c r="D49" s="3"/>
       <c r="E49" s="1"/>
       <c r="F49" s="1"/>
       <c r="G49" s="1"/>
@@ -3942,7 +3932,7 @@
       <c r="A50" s="1"/>
       <c r="B50" s="19"/>
       <c r="C50" s="23"/>
-      <c r="D50" s="54"/>
+      <c r="D50" s="3"/>
       <c r="E50" s="1"/>
       <c r="F50" s="1"/>
       <c r="G50" s="1"/>
@@ -3960,7 +3950,7 @@
       <c r="A51" s="1"/>
       <c r="B51" s="19"/>
       <c r="C51" s="23"/>
-      <c r="D51" s="54"/>
+      <c r="D51" s="3"/>
       <c r="E51" s="1"/>
       <c r="F51" s="1"/>
       <c r="G51" s="1"/>
@@ -3978,7 +3968,7 @@
       <c r="A52" s="1"/>
       <c r="B52" s="19"/>
       <c r="C52" s="23"/>
-      <c r="D52" s="54"/>
+      <c r="D52" s="3"/>
       <c r="E52" s="1"/>
       <c r="F52" s="1"/>
       <c r="G52" s="1"/>
@@ -3996,7 +3986,7 @@
       <c r="A53" s="1"/>
       <c r="B53" s="19"/>
       <c r="C53" s="23"/>
-      <c r="D53" s="54"/>
+      <c r="D53" s="3"/>
       <c r="E53" s="1"/>
       <c r="F53" s="1"/>
       <c r="G53" s="1"/>
@@ -4014,7 +4004,7 @@
       <c r="A54" s="1"/>
       <c r="B54" s="19"/>
       <c r="C54" s="23"/>
-      <c r="D54" s="54"/>
+      <c r="D54" s="3"/>
       <c r="E54" s="1"/>
       <c r="F54" s="1"/>
       <c r="G54" s="1"/>
@@ -4032,7 +4022,7 @@
       <c r="A55" s="1"/>
       <c r="B55" s="19"/>
       <c r="C55" s="23"/>
-      <c r="D55" s="54"/>
+      <c r="D55" s="3"/>
       <c r="E55" s="1"/>
       <c r="F55" s="1"/>
       <c r="G55" s="1"/>
@@ -4050,7 +4040,7 @@
       <c r="A56" s="1"/>
       <c r="B56" s="19"/>
       <c r="C56" s="23"/>
-      <c r="D56" s="54"/>
+      <c r="D56" s="3"/>
       <c r="E56" s="1"/>
       <c r="F56" s="1"/>
       <c r="G56" s="1"/>
@@ -4068,7 +4058,7 @@
       <c r="A57" s="1"/>
       <c r="B57" s="19"/>
       <c r="C57" s="23"/>
-      <c r="D57" s="54"/>
+      <c r="D57" s="3"/>
       <c r="E57" s="1"/>
       <c r="F57" s="1"/>
       <c r="G57" s="1"/>
@@ -4086,7 +4076,7 @@
       <c r="A58" s="1"/>
       <c r="B58" s="19"/>
       <c r="C58" s="23"/>
-      <c r="D58" s="54"/>
+      <c r="D58" s="3"/>
       <c r="E58" s="1"/>
       <c r="F58" s="1"/>
       <c r="G58" s="1"/>
@@ -4104,7 +4094,7 @@
       <c r="A59" s="1"/>
       <c r="B59" s="19"/>
       <c r="C59" s="23"/>
-      <c r="D59" s="54"/>
+      <c r="D59" s="3"/>
       <c r="E59" s="1"/>
       <c r="F59" s="1"/>
       <c r="G59" s="1"/>
@@ -4122,7 +4112,7 @@
       <c r="A60" s="1"/>
       <c r="B60" s="19"/>
       <c r="C60" s="23"/>
-      <c r="D60" s="54"/>
+      <c r="D60" s="3"/>
       <c r="E60" s="1"/>
       <c r="F60" s="1"/>
       <c r="G60" s="1"/>
@@ -4140,7 +4130,7 @@
       <c r="A61" s="1"/>
       <c r="B61" s="19"/>
       <c r="C61" s="23"/>
-      <c r="D61" s="54"/>
+      <c r="D61" s="3"/>
       <c r="E61" s="1"/>
       <c r="F61" s="1"/>
       <c r="G61" s="1"/>
@@ -4158,7 +4148,7 @@
       <c r="A62" s="1"/>
       <c r="B62" s="19"/>
       <c r="C62" s="23"/>
-      <c r="D62" s="54"/>
+      <c r="D62" s="3"/>
       <c r="E62" s="1"/>
       <c r="F62" s="1"/>
       <c r="G62" s="1"/>
@@ -4176,7 +4166,7 @@
       <c r="A63" s="1"/>
       <c r="B63" s="19"/>
       <c r="C63" s="23"/>
-      <c r="D63" s="54"/>
+      <c r="D63" s="3"/>
       <c r="E63" s="1"/>
       <c r="F63" s="1"/>
       <c r="G63" s="1"/>
@@ -4194,7 +4184,7 @@
       <c r="A64" s="1"/>
       <c r="B64" s="19"/>
       <c r="C64" s="23"/>
-      <c r="D64" s="54"/>
+      <c r="D64" s="3"/>
       <c r="E64" s="1"/>
       <c r="F64" s="1"/>
       <c r="G64" s="1"/>
@@ -4212,7 +4202,7 @@
       <c r="A65" s="1"/>
       <c r="B65" s="19"/>
       <c r="C65" s="23"/>
-      <c r="D65" s="54"/>
+      <c r="D65" s="3"/>
       <c r="E65" s="1"/>
       <c r="F65" s="1"/>
       <c r="G65" s="1"/>
@@ -4230,7 +4220,7 @@
       <c r="A66" s="1"/>
       <c r="B66" s="19"/>
       <c r="C66" s="23"/>
-      <c r="D66" s="54"/>
+      <c r="D66" s="3"/>
       <c r="E66" s="1"/>
       <c r="F66" s="1"/>
       <c r="G66" s="1"/>
@@ -4248,7 +4238,7 @@
       <c r="A67" s="1"/>
       <c r="B67" s="19"/>
       <c r="C67" s="23"/>
-      <c r="D67" s="54"/>
+      <c r="D67" s="3"/>
       <c r="E67" s="1"/>
       <c r="F67" s="1"/>
       <c r="G67" s="1"/>
@@ -4266,7 +4256,7 @@
       <c r="A68" s="1"/>
       <c r="B68" s="19"/>
       <c r="C68" s="23"/>
-      <c r="D68" s="54"/>
+      <c r="D68" s="3"/>
       <c r="E68" s="1"/>
       <c r="F68" s="1"/>
       <c r="G68" s="1"/>
@@ -4284,7 +4274,7 @@
       <c r="A69" s="1"/>
       <c r="B69" s="19"/>
       <c r="C69" s="23"/>
-      <c r="D69" s="54"/>
+      <c r="D69" s="3"/>
       <c r="E69" s="1"/>
       <c r="F69" s="1"/>
       <c r="G69" s="1"/>
@@ -4302,7 +4292,7 @@
       <c r="A70" s="1"/>
       <c r="B70" s="19"/>
       <c r="C70" s="23"/>
-      <c r="D70" s="54"/>
+      <c r="D70" s="3"/>
       <c r="E70" s="1"/>
       <c r="F70" s="1"/>
       <c r="G70" s="1"/>
@@ -4320,7 +4310,7 @@
       <c r="A71" s="1"/>
       <c r="B71" s="19"/>
       <c r="C71" s="23"/>
-      <c r="D71" s="54"/>
+      <c r="D71" s="3"/>
       <c r="E71" s="1"/>
       <c r="F71" s="1"/>
       <c r="G71" s="1"/>
@@ -4338,7 +4328,7 @@
       <c r="A72" s="1"/>
       <c r="B72" s="19"/>
       <c r="C72" s="23"/>
-      <c r="D72" s="54"/>
+      <c r="D72" s="3"/>
       <c r="E72" s="1"/>
       <c r="F72" s="1"/>
       <c r="G72" s="1"/>
@@ -4356,7 +4346,7 @@
       <c r="A73" s="1"/>
       <c r="B73" s="19"/>
       <c r="C73" s="23"/>
-      <c r="D73" s="54"/>
+      <c r="D73" s="3"/>
       <c r="E73" s="1"/>
       <c r="F73" s="1"/>
       <c r="G73" s="1"/>
@@ -4374,7 +4364,7 @@
       <c r="A74" s="1"/>
       <c r="B74" s="19"/>
       <c r="C74" s="23"/>
-      <c r="D74" s="54"/>
+      <c r="D74" s="3"/>
       <c r="E74" s="1"/>
       <c r="F74" s="1"/>
       <c r="G74" s="1"/>
@@ -4392,7 +4382,7 @@
       <c r="A75" s="1"/>
       <c r="B75" s="19"/>
       <c r="C75" s="23"/>
-      <c r="D75" s="54"/>
+      <c r="D75" s="3"/>
       <c r="E75" s="1"/>
       <c r="F75" s="1"/>
       <c r="G75" s="1"/>
@@ -4410,7 +4400,7 @@
       <c r="A76" s="1"/>
       <c r="B76" s="19"/>
       <c r="C76" s="23"/>
-      <c r="D76" s="54"/>
+      <c r="D76" s="3"/>
       <c r="E76" s="1"/>
       <c r="F76" s="1"/>
       <c r="G76" s="1"/>
@@ -4428,7 +4418,7 @@
       <c r="A77" s="1"/>
       <c r="B77" s="19"/>
       <c r="C77" s="23"/>
-      <c r="D77" s="54"/>
+      <c r="D77" s="3"/>
       <c r="E77" s="1"/>
       <c r="F77" s="1"/>
       <c r="G77" s="1"/>
@@ -4446,7 +4436,7 @@
       <c r="A78" s="1"/>
       <c r="B78" s="19"/>
       <c r="C78" s="23"/>
-      <c r="D78" s="54"/>
+      <c r="D78" s="3"/>
       <c r="E78" s="1"/>
       <c r="F78" s="1"/>
       <c r="G78" s="1"/>
@@ -4464,7 +4454,7 @@
       <c r="A79" s="1"/>
       <c r="B79" s="19"/>
       <c r="C79" s="23"/>
-      <c r="D79" s="54"/>
+      <c r="D79" s="3"/>
       <c r="E79" s="1"/>
       <c r="F79" s="1"/>
       <c r="G79" s="1"/>

</xml_diff>

<commit_message>
Some more exploring the data and visualizing
</commit_message>
<xml_diff>
--- a/Time_Tracking.xlsx
+++ b/Time_Tracking.xlsx
@@ -3128,7 +3128,9 @@
       <c r="C11" s="42" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="11"/>
+      <c r="D11" s="11">
+        <v>3.5</v>
+      </c>
       <c r="E11" s="39"/>
       <c r="F11" s="11"/>
       <c r="G11" s="39"/>
@@ -3150,7 +3152,9 @@
       <c r="C12" s="42" t="s">
         <v>20</v>
       </c>
-      <c r="D12" s="11"/>
+      <c r="D12" s="11">
+        <v>8</v>
+      </c>
       <c r="E12" s="39"/>
       <c r="F12" s="11"/>
       <c r="G12" s="39"/>

</xml_diff>

<commit_message>
Some more exploring and visualizing
</commit_message>
<xml_diff>
--- a/Time_Tracking.xlsx
+++ b/Time_Tracking.xlsx
@@ -3176,7 +3176,9 @@
       <c r="C13" s="42" t="s">
         <v>21</v>
       </c>
-      <c r="D13" s="11"/>
+      <c r="D13" s="11">
+        <v>7.5</v>
+      </c>
       <c r="E13" s="39"/>
       <c r="F13" s="11"/>
       <c r="G13" s="39"/>
@@ -3716,7 +3718,7 @@
       <c r="O37" s="3"/>
       <c r="P37" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="38" customHeight="1" ht="19.5">
       <c r="A38" s="1"/>
       <c r="B38" s="19"/>
       <c r="C38" s="23"/>
@@ -3734,7 +3736,7 @@
       <c r="O38" s="3"/>
       <c r="P38" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="39" customHeight="1" ht="19.5">
       <c r="A39" s="1"/>
       <c r="B39" s="19"/>
       <c r="C39" s="23"/>
@@ -3752,7 +3754,7 @@
       <c r="O39" s="3"/>
       <c r="P39" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="40" customHeight="1" ht="19.5">
       <c r="A40" s="1"/>
       <c r="B40" s="19"/>
       <c r="C40" s="23"/>
@@ -3770,7 +3772,7 @@
       <c r="O40" s="3"/>
       <c r="P40" s="3"/>
     </row>
-    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="18.75">
+    <row x14ac:dyDescent="0.25" r="41" customHeight="1" ht="19.5">
       <c r="A41" s="1"/>
       <c r="B41" s="19"/>
       <c r="C41" s="23"/>

</xml_diff>

<commit_message>
Updated all visualizations and added some more
</commit_message>
<xml_diff>
--- a/Time_Tracking.xlsx
+++ b/Time_Tracking.xlsx
@@ -3177,7 +3177,7 @@
         <v>21</v>
       </c>
       <c r="D13" s="11">
-        <v>7.5</v>
+        <v>6.5</v>
       </c>
       <c r="E13" s="39"/>
       <c r="F13" s="11"/>
@@ -3200,7 +3200,9 @@
       <c r="C14" s="42" t="s">
         <v>22</v>
       </c>
-      <c r="D14" s="11"/>
+      <c r="D14" s="11">
+        <v>5</v>
+      </c>
       <c r="E14" s="39"/>
       <c r="F14" s="11"/>
       <c r="G14" s="39"/>
@@ -3222,7 +3224,9 @@
       <c r="C15" s="42" t="s">
         <v>23</v>
       </c>
-      <c r="D15" s="11"/>
+      <c r="D15" s="11">
+        <v>7</v>
+      </c>
       <c r="E15" s="39"/>
       <c r="F15" s="11"/>
       <c r="G15" s="39"/>

</xml_diff>

<commit_message>
Update Git to match the server
</commit_message>
<xml_diff>
--- a/Time_Tracking.xlsx
+++ b/Time_Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekt-Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0A4A8BAC-E2CE-49AD-B1E0-FC5537B79F60}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717FAB45-7CAC-4460-8ED8-3B262507E465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oktober" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="335" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="41">
   <si>
     <t>Gesamtstunden</t>
   </si>
@@ -140,6 +140,30 @@
   <si>
     <t>Database Creation</t>
   </si>
+  <si>
+    <t>Creating csv files</t>
+  </si>
+  <si>
+    <t>Cleaning</t>
+  </si>
+  <si>
+    <t>Presentation, Cleaning</t>
+  </si>
+  <si>
+    <t>Feedback</t>
+  </si>
+  <si>
+    <t>Hypothesis finding</t>
+  </si>
+  <si>
+    <t>Milestone 2</t>
+  </si>
+  <si>
+    <t>Milestone 1</t>
+  </si>
+  <si>
+    <t>Hypothesis talk</t>
+  </si>
 </sst>
 </file>
 
@@ -211,7 +235,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="33">
+  <borders count="34">
     <border>
       <left/>
       <right/>
@@ -671,11 +695,26 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color rgb="FFC6C6C6"/>
+      </left>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="double">
+        <color rgb="FF000000"/>
+      </top>
+      <bottom style="medium">
+        <color rgb="FF000000"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="53">
+  <cellXfs count="55">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -825,6 +864,12 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="23" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="33" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1140,7 +1185,7 @@
   </sheetPr>
   <dimension ref="B1:G80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView topLeftCell="A14" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2660,7 +2705,7 @@
   <dimension ref="B1:G80"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="C27" sqref="C27"/>
+      <selection activeCell="D12" sqref="D12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2809,10 +2854,18 @@
       <c r="C11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="27"/>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>39</v>
+      </c>
+      <c r="F11" s="7">
+        <v>1</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>39</v>
+      </c>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="28">
@@ -3113,12 +3166,12 @@
       <c r="C36" s="46"/>
       <c r="D36" s="49" t="str">
         <f>"Ozan: "&amp;SUM(D5:D35)&amp;" Stunden"</f>
-        <v>Ozan: 5 Stunden</v>
+        <v>Ozan: 6 Stunden</v>
       </c>
       <c r="E36" s="48"/>
       <c r="F36" s="49" t="str">
         <f>"Tony: "&amp;SUM(F5:F35)&amp;" Stunden"</f>
-        <v>Tony: 2,5 Stunden</v>
+        <v>Tony: 3,5 Stunden</v>
       </c>
       <c r="G36" s="50"/>
     </row>
@@ -3319,8 +3372,8 @@
   </sheetPr>
   <dimension ref="B1:G80"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="E22" sqref="E22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3338,7 +3391,7 @@
       <c r="B1" s="16"/>
       <c r="C1" s="18"/>
     </row>
-    <row r="2" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="2:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.4">
       <c r="B2" s="36" t="s">
         <v>7</v>
       </c>
@@ -3348,7 +3401,7 @@
       <c r="F2" s="37"/>
       <c r="G2" s="39"/>
     </row>
-    <row r="3" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="2:7" ht="18.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B3" s="40" t="s">
         <v>12</v>
       </c>
@@ -3357,12 +3410,12 @@
         <v>2</v>
       </c>
       <c r="E3" s="41"/>
-      <c r="F3" s="43" t="s">
+      <c r="F3" s="51" t="s">
         <v>3</v>
       </c>
-      <c r="G3" s="44"/>
-    </row>
-    <row r="4" spans="2:7" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="G3" s="52"/>
+    </row>
+    <row r="4" spans="2:7" ht="18.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="19" t="s">
         <v>12</v>
       </c>
@@ -3489,8 +3542,12 @@
       <c r="C12" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="26"/>
+      <c r="D12" s="7">
+        <v>8</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>30</v>
+      </c>
       <c r="F12" s="7"/>
       <c r="G12" s="27"/>
     </row>
@@ -3501,8 +3558,12 @@
       <c r="C13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="26"/>
+      <c r="D13" s="7">
+        <v>10</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>33</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="27"/>
     </row>
@@ -3513,8 +3574,12 @@
       <c r="C14" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="26"/>
+      <c r="D14" s="7">
+        <v>11</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>34</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="27"/>
     </row>
@@ -3525,10 +3590,18 @@
       <c r="C15" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D15" s="7"/>
-      <c r="E15" s="26"/>
-      <c r="F15" s="7"/>
-      <c r="G15" s="27"/>
+      <c r="D15" s="7">
+        <v>12</v>
+      </c>
+      <c r="E15" s="26" t="s">
+        <v>34</v>
+      </c>
+      <c r="F15" s="7">
+        <v>6</v>
+      </c>
+      <c r="G15" s="27" t="s">
+        <v>34</v>
+      </c>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B16" s="28">
@@ -3537,10 +3610,18 @@
       <c r="C16" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="26"/>
-      <c r="F16" s="7"/>
-      <c r="G16" s="27"/>
+      <c r="D16" s="7">
+        <v>11</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F16" s="7">
+        <v>6</v>
+      </c>
+      <c r="G16" s="27" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B17" s="28">
@@ -3549,10 +3630,18 @@
       <c r="C17" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="26"/>
-      <c r="F17" s="7"/>
-      <c r="G17" s="27"/>
+      <c r="D17" s="7">
+        <v>9</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>35</v>
+      </c>
+      <c r="F17" s="7">
+        <v>8</v>
+      </c>
+      <c r="G17" s="27" t="s">
+        <v>35</v>
+      </c>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B18" s="28">
@@ -3573,10 +3662,18 @@
       <c r="C19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="26"/>
-      <c r="F19" s="7"/>
-      <c r="G19" s="27"/>
+      <c r="D19" s="7">
+        <v>1</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>38</v>
+      </c>
+      <c r="F19" s="7">
+        <v>1</v>
+      </c>
+      <c r="G19" s="27" t="s">
+        <v>38</v>
+      </c>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B20" s="28">
@@ -3587,8 +3684,12 @@
       </c>
       <c r="D20" s="7"/>
       <c r="E20" s="26"/>
-      <c r="F20" s="7"/>
-      <c r="G20" s="27"/>
+      <c r="F20" s="7">
+        <v>3</v>
+      </c>
+      <c r="G20" s="27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B21" s="28">
@@ -3597,10 +3698,18 @@
       <c r="C21" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="26"/>
-      <c r="F21" s="7"/>
-      <c r="G21" s="27"/>
+      <c r="D21" s="7">
+        <v>1</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F21" s="7">
+        <v>1</v>
+      </c>
+      <c r="G21" s="27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B22" s="28">
@@ -3633,8 +3742,12 @@
       <c r="C24" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="26"/>
+      <c r="D24" s="7">
+        <v>8</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>36</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="27"/>
     </row>
@@ -3645,8 +3758,12 @@
       <c r="C25" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="26"/>
+      <c r="D25" s="7">
+        <v>9</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>36</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="27"/>
     </row>
@@ -3659,8 +3776,12 @@
       </c>
       <c r="D26" s="7"/>
       <c r="E26" s="26"/>
-      <c r="F26" s="7"/>
-      <c r="G26" s="27"/>
+      <c r="F26" s="7">
+        <v>4</v>
+      </c>
+      <c r="G26" s="27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B27" s="28">
@@ -3669,10 +3790,18 @@
       <c r="C27" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="26"/>
-      <c r="F27" s="7"/>
-      <c r="G27" s="27"/>
+      <c r="D27" s="7">
+        <v>1</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F27" s="7">
+        <v>1</v>
+      </c>
+      <c r="G27" s="27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B28" s="28">
@@ -3683,8 +3812,12 @@
       </c>
       <c r="D28" s="7"/>
       <c r="E28" s="26"/>
-      <c r="F28" s="7"/>
-      <c r="G28" s="27"/>
+      <c r="F28" s="7">
+        <v>4</v>
+      </c>
+      <c r="G28" s="27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B29" s="28">
@@ -3693,10 +3826,18 @@
       <c r="C29" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="26"/>
-      <c r="F29" s="7"/>
-      <c r="G29" s="27"/>
+      <c r="D29" s="7">
+        <v>1</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F29" s="7">
+        <v>1</v>
+      </c>
+      <c r="G29" s="27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="30" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B30" s="28">
@@ -3717,8 +3858,12 @@
       <c r="C31" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="26"/>
+      <c r="D31" s="7">
+        <v>6</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>36</v>
+      </c>
       <c r="F31" s="7"/>
       <c r="G31" s="27"/>
     </row>
@@ -3729,8 +3874,12 @@
       <c r="C32" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="26"/>
+      <c r="D32" s="7">
+        <v>7</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>36</v>
+      </c>
       <c r="F32" s="7"/>
       <c r="G32" s="27"/>
     </row>
@@ -3777,12 +3926,12 @@
       <c r="C36" s="46"/>
       <c r="D36" s="49" t="str">
         <f>"Ozan: "&amp;SUM(D5:D35)&amp;" Stunden"</f>
-        <v>Ozan: 25 Stunden</v>
+        <v>Ozan: 120 Stunden</v>
       </c>
       <c r="E36" s="48"/>
       <c r="F36" s="49" t="str">
         <f>"Tony: "&amp;SUM(F5:F35)&amp;" Stunden"</f>
-        <v>Tony: 0 Stunden</v>
+        <v>Tony: 35 Stunden</v>
       </c>
       <c r="G36" s="50"/>
     </row>
@@ -3983,7 +4132,9 @@
   </sheetPr>
   <dimension ref="B1:G78"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4051,8 +4202,12 @@
       <c r="C5" s="25" t="s">
         <v>19</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="26"/>
+      <c r="D5" s="7">
+        <v>3</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>37</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="27"/>
     </row>
@@ -4075,8 +4230,12 @@
       <c r="C7" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="7">
+        <v>6</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>37</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="27"/>
     </row>
@@ -4087,10 +4246,18 @@
       <c r="C8" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="26"/>
-      <c r="F8" s="7"/>
-      <c r="G8" s="27"/>
+      <c r="D8" s="7">
+        <v>8</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F8" s="7">
+        <v>5</v>
+      </c>
+      <c r="G8" s="27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B9" s="28">
@@ -4099,10 +4266,18 @@
       <c r="C9" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="26"/>
-      <c r="F9" s="7"/>
-      <c r="G9" s="27"/>
+      <c r="D9" s="7">
+        <v>8</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>37</v>
+      </c>
+      <c r="F9" s="7">
+        <v>4</v>
+      </c>
+      <c r="G9" s="27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B10" s="28">
@@ -4111,8 +4286,12 @@
       <c r="C10" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="26"/>
+      <c r="D10" s="7">
+        <v>9</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>37</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="27"/>
     </row>
@@ -4123,10 +4302,18 @@
       <c r="C11" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="26"/>
-      <c r="F11" s="7"/>
-      <c r="G11" s="27"/>
+      <c r="D11" s="7">
+        <v>10</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>25</v>
+      </c>
+      <c r="F11" s="7">
+        <v>8</v>
+      </c>
+      <c r="G11" s="27" t="s">
+        <v>37</v>
+      </c>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B12" s="28">
@@ -4399,12 +4586,12 @@
       <c r="C34" s="46"/>
       <c r="D34" s="49" t="str">
         <f>"Ozan: "&amp;SUM(D5:D33)&amp;" Stunden"</f>
-        <v>Ozan: 0 Stunden</v>
+        <v>Ozan: 44 Stunden</v>
       </c>
       <c r="E34" s="48"/>
       <c r="F34" s="49" t="str">
         <f>"Tony: "&amp;SUM(F5:F33)&amp;" Stunden"</f>
-        <v>Tony: 0 Stunden</v>
+        <v>Tony: 17 Stunden</v>
       </c>
       <c r="G34" s="50"/>
     </row>
@@ -5885,7 +6072,9 @@
   </sheetPr>
   <dimension ref="B1:D55"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5910,11 +6099,11 @@
       <c r="D3" s="2"/>
     </row>
     <row r="4" spans="2:4" ht="24.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="51" t="s">
+      <c r="B4" s="53" t="s">
         <v>0</v>
       </c>
       <c r="C4" s="38"/>
-      <c r="D4" s="52"/>
+      <c r="D4" s="54"/>
     </row>
     <row r="5" spans="2:4" ht="20.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" s="3" t="s">
@@ -5959,11 +6148,11 @@
       </c>
       <c r="C8" s="7">
         <f>SUM(Dezember!D5:D35)</f>
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="D8" s="8">
         <f>SUM(Dezember!F5:F35)</f>
-        <v>2.5</v>
+        <v>3.5</v>
       </c>
     </row>
     <row r="9" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5972,11 +6161,11 @@
       </c>
       <c r="C9" s="7">
         <f>SUM(Januar!D5:D35)</f>
-        <v>25</v>
+        <v>120</v>
       </c>
       <c r="D9" s="8">
         <f>SUM(Januar!F5:F35)</f>
-        <v>0</v>
+        <v>35</v>
       </c>
     </row>
     <row r="10" spans="2:4" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -5985,11 +6174,11 @@
       </c>
       <c r="C10" s="7">
         <f>SUM(Februar!D5:D33)</f>
-        <v>0</v>
+        <v>44</v>
       </c>
       <c r="D10" s="8">
         <f>SUM(Februar!F5:F33)</f>
-        <v>0</v>
+        <v>17</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6024,11 +6213,11 @@
       </c>
       <c r="C13" s="12" t="str">
         <f>SUM(C6:C12)&amp;" Stunden"</f>
-        <v>91 Stunden</v>
+        <v>231 Stunden</v>
       </c>
       <c r="D13" s="13" t="str">
         <f>SUM(D6:D12)&amp;" Stunden"</f>
-        <v>40,5 Stunden</v>
+        <v>93,5 Stunden</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Final (and overdue) Commit
</commit_message>
<xml_diff>
--- a/Time_Tracking.xlsx
+++ b/Time_Tracking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27231"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27425"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\Projekt-Data-Science\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{717FAB45-7CAC-4460-8ED8-3B262507E465}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A4B7510-4CCE-47F1-BC0D-84598A7F1366}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Oktober" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="370" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="407" uniqueCount="50">
   <si>
     <t>Gesamtstunden</t>
   </si>
@@ -120,9 +120,6 @@
     <t>Presentation</t>
   </si>
   <si>
-    <t>Worked in Feedback</t>
-  </si>
-  <si>
     <t>Setup Discord/Excel</t>
   </si>
   <si>
@@ -163,6 +160,36 @@
   </si>
   <si>
     <t>Hypothesis talk</t>
+  </si>
+  <si>
+    <t>Pitch</t>
+  </si>
+  <si>
+    <t>Cleaning again</t>
+  </si>
+  <si>
+    <t>Hypothesis 1</t>
+  </si>
+  <si>
+    <t>Hypothesis 2</t>
+  </si>
+  <si>
+    <t>Cleaning final</t>
+  </si>
+  <si>
+    <t>Milestone 3</t>
+  </si>
+  <si>
+    <t>External cleaning</t>
+  </si>
+  <si>
+    <t>Report</t>
+  </si>
+  <si>
+    <t>Paper</t>
+  </si>
+  <si>
+    <t>Presentation &amp; Poster</t>
   </si>
 </sst>
 </file>
@@ -714,7 +741,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="55">
+  <cellXfs count="57">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="4" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -877,6 +904,12 @@
     </xf>
     <xf numFmtId="4" fontId="2" fillId="2" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="4" fontId="4" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="26" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1185,7 +1218,7 @@
   </sheetPr>
   <dimension ref="B1:G80"/>
   <sheetViews>
-    <sheetView topLeftCell="A14" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -1570,7 +1603,7 @@
         <v>5</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="27"/>
@@ -1880,7 +1913,9 @@
   </sheetPr>
   <dimension ref="B1:G79"/>
   <sheetViews>
-    <sheetView topLeftCell="A7" workbookViewId="0"/>
+    <sheetView topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E32" sqref="E32"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -2338,10 +2373,10 @@
       <c r="C30" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D30" s="7">
+      <c r="D30" s="55">
         <v>3</v>
       </c>
-      <c r="E30" s="26" t="s">
+      <c r="E30" s="56" t="s">
         <v>24</v>
       </c>
       <c r="F30" s="7">
@@ -2374,7 +2409,7 @@
         <v>1.5</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="27"/>
@@ -2705,7 +2740,7 @@
   <dimension ref="B1:G80"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="G21" sqref="G21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -2838,13 +2873,13 @@
         <v>2.5</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F10" s="7">
         <v>2.5</v>
       </c>
       <c r="G10" s="27" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="11" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -2854,17 +2889,17 @@
       <c r="C11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7">
+      <c r="D11" s="55">
         <v>1</v>
       </c>
-      <c r="E11" s="26" t="s">
-        <v>39</v>
+      <c r="E11" s="56" t="s">
+        <v>38</v>
       </c>
       <c r="F11" s="7">
         <v>1</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3010,7 +3045,7 @@
         <v>2.5</v>
       </c>
       <c r="E23" s="26" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F23" s="7"/>
       <c r="G23" s="27"/>
@@ -3373,7 +3408,7 @@
   <dimension ref="B1:G80"/>
   <sheetViews>
     <sheetView topLeftCell="A3" workbookViewId="0">
-      <selection activeCell="E22" sqref="E22"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3482,7 +3517,7 @@
         <v>4</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="F8" s="7"/>
       <c r="G8" s="27"/>
@@ -3498,7 +3533,7 @@
         <v>8</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F9" s="7"/>
       <c r="G9" s="27"/>
@@ -3514,7 +3549,7 @@
         <v>4</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="27"/>
@@ -3530,7 +3565,7 @@
         <v>9</v>
       </c>
       <c r="E11" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F11" s="7"/>
       <c r="G11" s="27"/>
@@ -3546,7 +3581,7 @@
         <v>8</v>
       </c>
       <c r="E12" s="26" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F12" s="7"/>
       <c r="G12" s="27"/>
@@ -3562,7 +3597,7 @@
         <v>10</v>
       </c>
       <c r="E13" s="26" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="F13" s="7"/>
       <c r="G13" s="27"/>
@@ -3578,7 +3613,7 @@
         <v>11</v>
       </c>
       <c r="E14" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F14" s="7"/>
       <c r="G14" s="27"/>
@@ -3594,13 +3629,13 @@
         <v>12</v>
       </c>
       <c r="E15" s="26" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="F15" s="7">
         <v>6</v>
       </c>
       <c r="G15" s="27" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="16" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3614,13 +3649,13 @@
         <v>11</v>
       </c>
       <c r="E16" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F16" s="7">
         <v>6</v>
       </c>
       <c r="G16" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="17" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3634,13 +3669,13 @@
         <v>9</v>
       </c>
       <c r="E17" s="26" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="F17" s="7">
         <v>8</v>
       </c>
       <c r="G17" s="27" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="18" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3662,17 +3697,17 @@
       <c r="C19" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D19" s="7">
+      <c r="D19" s="55">
         <v>1</v>
       </c>
-      <c r="E19" s="26" t="s">
-        <v>38</v>
+      <c r="E19" s="56" t="s">
+        <v>37</v>
       </c>
       <c r="F19" s="7">
         <v>1</v>
       </c>
       <c r="G19" s="27" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="20" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3688,7 +3723,7 @@
         <v>3</v>
       </c>
       <c r="G20" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="21" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3702,13 +3737,13 @@
         <v>1</v>
       </c>
       <c r="E21" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F21" s="7">
         <v>1</v>
       </c>
       <c r="G21" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="22" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3746,7 +3781,7 @@
         <v>8</v>
       </c>
       <c r="E24" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F24" s="7"/>
       <c r="G24" s="27"/>
@@ -3762,7 +3797,7 @@
         <v>9</v>
       </c>
       <c r="E25" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F25" s="7"/>
       <c r="G25" s="27"/>
@@ -3780,7 +3815,7 @@
         <v>4</v>
       </c>
       <c r="G26" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="27" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3794,13 +3829,13 @@
         <v>1</v>
       </c>
       <c r="E27" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F27" s="7">
         <v>1</v>
       </c>
       <c r="G27" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="28" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3816,7 +3851,7 @@
         <v>4</v>
       </c>
       <c r="G28" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="29" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3830,13 +3865,13 @@
         <v>1</v>
       </c>
       <c r="E29" s="26" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F29" s="7">
         <v>1</v>
       </c>
       <c r="G29" s="27" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="30" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -3862,7 +3897,7 @@
         <v>6</v>
       </c>
       <c r="E31" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F31" s="7"/>
       <c r="G31" s="27"/>
@@ -3878,7 +3913,7 @@
         <v>7</v>
       </c>
       <c r="E32" s="26" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F32" s="7"/>
       <c r="G32" s="27"/>
@@ -4132,8 +4167,8 @@
   </sheetPr>
   <dimension ref="B1:G78"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -4206,7 +4241,7 @@
         <v>3</v>
       </c>
       <c r="E5" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F5" s="7"/>
       <c r="G5" s="27"/>
@@ -4234,7 +4269,7 @@
         <v>6</v>
       </c>
       <c r="E7" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F7" s="7"/>
       <c r="G7" s="27"/>
@@ -4250,13 +4285,13 @@
         <v>8</v>
       </c>
       <c r="E8" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="7">
         <v>5</v>
       </c>
       <c r="G8" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="9" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4270,13 +4305,13 @@
         <v>8</v>
       </c>
       <c r="E9" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F9" s="7">
         <v>4</v>
       </c>
       <c r="G9" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="10" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4290,7 +4325,7 @@
         <v>9</v>
       </c>
       <c r="E10" s="26" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F10" s="7"/>
       <c r="G10" s="27"/>
@@ -4312,7 +4347,7 @@
         <v>8</v>
       </c>
       <c r="G11" s="27" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="12" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
@@ -4322,10 +4357,18 @@
       <c r="C12" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D12" s="7"/>
-      <c r="E12" s="26"/>
-      <c r="F12" s="7"/>
-      <c r="G12" s="27"/>
+      <c r="D12" s="7">
+        <v>1</v>
+      </c>
+      <c r="E12" s="26" t="s">
+        <v>40</v>
+      </c>
+      <c r="F12" s="7">
+        <v>1</v>
+      </c>
+      <c r="G12" s="27" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="13" spans="2:7" ht="15" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B13" s="28">
@@ -4334,8 +4377,12 @@
       <c r="C13" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="26"/>
+      <c r="D13" s="7">
+        <v>4</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="27"/>
     </row>
@@ -4346,8 +4393,12 @@
       <c r="C14" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D14" s="7"/>
-      <c r="E14" s="26"/>
+      <c r="D14" s="7">
+        <v>5</v>
+      </c>
+      <c r="E14" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="F14" s="7"/>
       <c r="G14" s="27"/>
     </row>
@@ -4406,8 +4457,12 @@
       <c r="C19" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D19" s="7"/>
-      <c r="E19" s="26"/>
+      <c r="D19" s="7">
+        <v>3</v>
+      </c>
+      <c r="E19" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="F19" s="7"/>
       <c r="G19" s="27"/>
     </row>
@@ -4430,8 +4485,12 @@
       <c r="C21" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D21" s="7"/>
-      <c r="E21" s="26"/>
+      <c r="D21" s="7">
+        <v>3</v>
+      </c>
+      <c r="E21" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="F21" s="7"/>
       <c r="G21" s="27"/>
     </row>
@@ -4442,8 +4501,12 @@
       <c r="C22" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D22" s="7"/>
-      <c r="E22" s="26"/>
+      <c r="D22" s="7">
+        <v>4</v>
+      </c>
+      <c r="E22" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="F22" s="7"/>
       <c r="G22" s="27"/>
     </row>
@@ -4454,8 +4517,12 @@
       <c r="C23" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D23" s="7"/>
-      <c r="E23" s="26"/>
+      <c r="D23" s="55">
+        <v>1</v>
+      </c>
+      <c r="E23" s="56" t="s">
+        <v>45</v>
+      </c>
       <c r="F23" s="7"/>
       <c r="G23" s="27"/>
     </row>
@@ -4466,8 +4533,12 @@
       <c r="C24" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="26"/>
+      <c r="D24" s="7">
+        <v>3</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="27"/>
     </row>
@@ -4478,8 +4549,12 @@
       <c r="C25" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="26"/>
+      <c r="D25" s="7">
+        <v>3</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="27"/>
     </row>
@@ -4502,8 +4577,12 @@
       <c r="C27" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D27" s="7"/>
-      <c r="E27" s="26"/>
+      <c r="D27" s="7">
+        <v>5</v>
+      </c>
+      <c r="E27" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="F27" s="7"/>
       <c r="G27" s="27"/>
     </row>
@@ -4514,8 +4593,12 @@
       <c r="C28" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D28" s="7"/>
-      <c r="E28" s="26"/>
+      <c r="D28" s="7">
+        <v>1</v>
+      </c>
+      <c r="E28" s="26" t="s">
+        <v>46</v>
+      </c>
       <c r="F28" s="7"/>
       <c r="G28" s="27"/>
     </row>
@@ -4526,8 +4609,12 @@
       <c r="C29" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D29" s="7"/>
-      <c r="E29" s="26"/>
+      <c r="D29" s="7">
+        <v>4</v>
+      </c>
+      <c r="E29" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="F29" s="7"/>
       <c r="G29" s="27"/>
     </row>
@@ -4538,8 +4625,12 @@
       <c r="C30" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="7"/>
-      <c r="E30" s="26"/>
+      <c r="D30" s="7">
+        <v>3</v>
+      </c>
+      <c r="E30" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="F30" s="7"/>
       <c r="G30" s="27"/>
     </row>
@@ -4550,8 +4641,12 @@
       <c r="C31" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D31" s="7"/>
-      <c r="E31" s="26"/>
+      <c r="D31" s="7">
+        <v>4</v>
+      </c>
+      <c r="E31" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="F31" s="7"/>
       <c r="G31" s="27"/>
     </row>
@@ -4562,8 +4657,12 @@
       <c r="C32" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D32" s="7"/>
-      <c r="E32" s="26"/>
+      <c r="D32" s="7">
+        <v>1</v>
+      </c>
+      <c r="E32" s="26" t="s">
+        <v>41</v>
+      </c>
       <c r="F32" s="7"/>
       <c r="G32" s="27"/>
     </row>
@@ -4574,8 +4673,12 @@
       <c r="C33" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D33" s="7"/>
-      <c r="E33" s="26"/>
+      <c r="D33" s="7">
+        <v>4</v>
+      </c>
+      <c r="E33" s="26" t="s">
+        <v>44</v>
+      </c>
       <c r="F33" s="7"/>
       <c r="G33" s="27"/>
     </row>
@@ -4586,12 +4689,12 @@
       <c r="C34" s="46"/>
       <c r="D34" s="49" t="str">
         <f>"Ozan: "&amp;SUM(D5:D33)&amp;" Stunden"</f>
-        <v>Ozan: 44 Stunden</v>
+        <v>Ozan: 93 Stunden</v>
       </c>
       <c r="E34" s="48"/>
       <c r="F34" s="49" t="str">
         <f>"Tony: "&amp;SUM(F5:F33)&amp;" Stunden"</f>
-        <v>Tony: 17 Stunden</v>
+        <v>Tony: 18 Stunden</v>
       </c>
       <c r="G34" s="50"/>
     </row>
@@ -4792,7 +4895,9 @@
   </sheetPr>
   <dimension ref="B1:G80"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E14" sqref="E14"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -4860,8 +4965,12 @@
       <c r="C5" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="D5" s="7"/>
-      <c r="E5" s="26"/>
+      <c r="D5" s="7">
+        <v>5</v>
+      </c>
+      <c r="E5" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="F5" s="7"/>
       <c r="G5" s="27"/>
     </row>
@@ -4872,8 +4981,12 @@
       <c r="C6" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D6" s="7"/>
-      <c r="E6" s="26"/>
+      <c r="D6" s="7">
+        <v>6</v>
+      </c>
+      <c r="E6" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="F6" s="7"/>
       <c r="G6" s="27"/>
     </row>
@@ -4884,8 +4997,12 @@
       <c r="C7" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D7" s="7"/>
-      <c r="E7" s="26"/>
+      <c r="D7" s="7">
+        <v>4</v>
+      </c>
+      <c r="E7" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="F7" s="7"/>
       <c r="G7" s="27"/>
     </row>
@@ -4896,8 +5013,12 @@
       <c r="C8" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="26"/>
+      <c r="D8" s="7">
+        <v>6</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>43</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="27"/>
     </row>
@@ -4908,8 +5029,12 @@
       <c r="C9" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="26"/>
+      <c r="D9" s="7">
+        <v>3</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>42</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="27"/>
     </row>
@@ -4920,8 +5045,12 @@
       <c r="C10" s="29" t="s">
         <v>18</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="26"/>
+      <c r="D10" s="7">
+        <v>8</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>25</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="27"/>
     </row>
@@ -4932,8 +5061,12 @@
       <c r="C11" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="26"/>
+      <c r="D11" s="7">
+        <v>1</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>47</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="27"/>
     </row>
@@ -5208,8 +5341,12 @@
       <c r="C34" s="34" t="s">
         <v>21</v>
       </c>
-      <c r="D34" s="7"/>
-      <c r="E34" s="26"/>
+      <c r="D34" s="7">
+        <v>6</v>
+      </c>
+      <c r="E34" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="F34" s="7"/>
       <c r="G34" s="27"/>
     </row>
@@ -5220,8 +5357,12 @@
       <c r="C35" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="D35" s="7"/>
-      <c r="E35" s="26"/>
+      <c r="D35" s="7">
+        <v>8</v>
+      </c>
+      <c r="E35" s="26" t="s">
+        <v>35</v>
+      </c>
       <c r="F35" s="7"/>
       <c r="G35" s="27"/>
     </row>
@@ -5232,7 +5373,7 @@
       <c r="C36" s="46"/>
       <c r="D36" s="49" t="str">
         <f>"Ozan: "&amp;SUM(D5:D35)&amp;" Stunden"</f>
-        <v>Ozan: 0 Stunden</v>
+        <v>Ozan: 47 Stunden</v>
       </c>
       <c r="E36" s="48"/>
       <c r="F36" s="49" t="str">
@@ -5438,7 +5579,9 @@
   </sheetPr>
   <dimension ref="B1:G79"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E29" sqref="E29"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -5542,8 +5685,12 @@
       <c r="C8" s="29" t="s">
         <v>19</v>
       </c>
-      <c r="D8" s="7"/>
-      <c r="E8" s="26"/>
+      <c r="D8" s="7">
+        <v>4</v>
+      </c>
+      <c r="E8" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F8" s="7"/>
       <c r="G8" s="27"/>
     </row>
@@ -5554,8 +5701,12 @@
       <c r="C9" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D9" s="7"/>
-      <c r="E9" s="26"/>
+      <c r="D9" s="7">
+        <v>3</v>
+      </c>
+      <c r="E9" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F9" s="7"/>
       <c r="G9" s="27"/>
     </row>
@@ -5566,8 +5717,12 @@
       <c r="C10" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D10" s="7"/>
-      <c r="E10" s="26"/>
+      <c r="D10" s="7">
+        <v>3</v>
+      </c>
+      <c r="E10" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F10" s="7"/>
       <c r="G10" s="27"/>
     </row>
@@ -5578,8 +5733,12 @@
       <c r="C11" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D11" s="7"/>
-      <c r="E11" s="26"/>
+      <c r="D11" s="7">
+        <v>4</v>
+      </c>
+      <c r="E11" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F11" s="7"/>
       <c r="G11" s="27"/>
     </row>
@@ -5602,8 +5761,12 @@
       <c r="C13" s="29" t="s">
         <v>17</v>
       </c>
-      <c r="D13" s="7"/>
-      <c r="E13" s="26"/>
+      <c r="D13" s="7">
+        <v>7</v>
+      </c>
+      <c r="E13" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F13" s="7"/>
       <c r="G13" s="27"/>
     </row>
@@ -5638,8 +5801,12 @@
       <c r="C16" s="29" t="s">
         <v>20</v>
       </c>
-      <c r="D16" s="7"/>
-      <c r="E16" s="26"/>
+      <c r="D16" s="7">
+        <v>10</v>
+      </c>
+      <c r="E16" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F16" s="7"/>
       <c r="G16" s="27"/>
     </row>
@@ -5650,8 +5817,12 @@
       <c r="C17" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D17" s="7"/>
-      <c r="E17" s="26"/>
+      <c r="D17" s="7">
+        <v>8</v>
+      </c>
+      <c r="E17" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F17" s="7"/>
       <c r="G17" s="27"/>
     </row>
@@ -5662,8 +5833,12 @@
       <c r="C18" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D18" s="7"/>
-      <c r="E18" s="26"/>
+      <c r="D18" s="7">
+        <v>7</v>
+      </c>
+      <c r="E18" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="F18" s="7"/>
       <c r="G18" s="27"/>
     </row>
@@ -5734,8 +5909,12 @@
       <c r="C24" s="29" t="s">
         <v>21</v>
       </c>
-      <c r="D24" s="7"/>
-      <c r="E24" s="26"/>
+      <c r="D24" s="7">
+        <v>5</v>
+      </c>
+      <c r="E24" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="F24" s="7"/>
       <c r="G24" s="27"/>
     </row>
@@ -5746,8 +5925,12 @@
       <c r="C25" s="29" t="s">
         <v>22</v>
       </c>
-      <c r="D25" s="7"/>
-      <c r="E25" s="26"/>
+      <c r="D25" s="7">
+        <v>8</v>
+      </c>
+      <c r="E25" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="F25" s="7"/>
       <c r="G25" s="27"/>
     </row>
@@ -5758,8 +5941,12 @@
       <c r="C26" s="29" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="7"/>
-      <c r="E26" s="26"/>
+      <c r="D26" s="7">
+        <v>10</v>
+      </c>
+      <c r="E26" s="26" t="s">
+        <v>49</v>
+      </c>
       <c r="F26" s="7"/>
       <c r="G26" s="27"/>
     </row>
@@ -5866,7 +6053,7 @@
       <c r="C35" s="46"/>
       <c r="D35" s="49" t="str">
         <f>"Ozan: "&amp;SUM(D5:D34)&amp;" Stunden"</f>
-        <v>Ozan: 0 Stunden</v>
+        <v>Ozan: 69 Stunden</v>
       </c>
       <c r="E35" s="48"/>
       <c r="F35" s="49" t="str">
@@ -6073,7 +6260,7 @@
   <dimension ref="B1:D55"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C13" sqref="C13"/>
+      <selection activeCell="F31" sqref="F31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6174,11 +6361,11 @@
       </c>
       <c r="C10" s="7">
         <f>SUM(Februar!D5:D33)</f>
-        <v>44</v>
+        <v>93</v>
       </c>
       <c r="D10" s="8">
         <f>SUM(Februar!F5:F33)</f>
-        <v>17</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -6187,7 +6374,7 @@
       </c>
       <c r="C11" s="7">
         <f>SUM(März!D5:D35)</f>
-        <v>0</v>
+        <v>47</v>
       </c>
       <c r="D11" s="8">
         <f>SUM(März!F5:F35)</f>
@@ -6200,7 +6387,7 @@
       </c>
       <c r="C12" s="7">
         <f>SUM(April!D5:D34)</f>
-        <v>0</v>
+        <v>69</v>
       </c>
       <c r="D12" s="8">
         <f>SUM(April!F5:F34)</f>
@@ -6213,11 +6400,11 @@
       </c>
       <c r="C13" s="12" t="str">
         <f>SUM(C6:C12)&amp;" Stunden"</f>
-        <v>231 Stunden</v>
+        <v>396 Stunden</v>
       </c>
       <c r="D13" s="13" t="str">
         <f>SUM(D6:D12)&amp;" Stunden"</f>
-        <v>93,5 Stunden</v>
+        <v>94,5 Stunden</v>
       </c>
     </row>
     <row r="14" spans="2:4" ht="18.75" customHeight="1" x14ac:dyDescent="0.25">

</xml_diff>